<commit_message>
Fixed Event Update Bug
Old Data does not stay when new data is saved.

Status Option cannot populate when displayed, but does give validation
warning when submitting.
</commit_message>
<xml_diff>
--- a/Supplier Email List.xlsx
+++ b/Supplier Email List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15920" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>Email</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>Replaced with CPalmer@bcipkg.com</t>
-  </si>
-  <si>
-    <t>UNKNOWN</t>
   </si>
 </sst>
 </file>
@@ -514,7 +511,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0"/>
@@ -637,7 +634,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3">

</xml_diff>